<commit_message>
Add the results from ALL the experiments.
</commit_message>
<xml_diff>
--- a/results/total_registration_results.xlsx
+++ b/results/total_registration_results.xlsx
@@ -439,11 +439,11 @@
   </sheetPr>
   <dimension ref="A1:K87"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F39" activeCellId="0" sqref="F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="0" width="11.52"/>

</xml_diff>